<commit_message>
added K_CSM and K_PSM results printing
</commit_message>
<xml_diff>
--- a/feasibility_flags_flat.xlsx
+++ b/feasibility_flags_flat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adevr\vol_smile_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB25EE4-EC82-4185-93A3-F5DAE336E6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECBB8A1-3275-45B5-913B-08F4BDC3C3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,55 +108,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>162721</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>76955</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBC74685-81E2-3481-595B-243F0CEB61E1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2990850" y="0"/>
-          <a:ext cx="5706271" cy="5410955"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -447,7 +398,7 @@
   <dimension ref="A1:D169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,7 +1422,7 @@
         <v>1.4</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1653,7 +1604,7 @@
         <v>0.8</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1667,7 +1618,7 @@
         <v>1</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1681,7 +1632,7 @@
         <v>1.2</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1695,7 +1646,7 @@
         <v>1.4</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,7 +1674,7 @@
         <v>1</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -1737,7 +1688,7 @@
         <v>1.2</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1751,7 +1702,7 @@
         <v>1.4</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -1779,7 +1730,7 @@
         <v>1</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -1793,7 +1744,7 @@
         <v>1.2</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1807,7 +1758,7 @@
         <v>1.4</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1835,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -1849,7 +1800,7 @@
         <v>1.2</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1863,7 +1814,7 @@
         <v>1.4</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -1905,7 +1856,7 @@
         <v>1.2</v>
       </c>
       <c r="D104">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -1919,7 +1870,7 @@
         <v>1.4</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -1961,7 +1912,7 @@
         <v>1.2</v>
       </c>
       <c r="D108">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -1975,7 +1926,7 @@
         <v>1.4</v>
       </c>
       <c r="D109">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2017,7 +1968,7 @@
         <v>1.2</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2031,7 +1982,7 @@
         <v>1.4</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2045,7 +1996,7 @@
         <v>0.8</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2059,7 +2010,7 @@
         <v>1</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2073,7 +2024,7 @@
         <v>1.2</v>
       </c>
       <c r="D116">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2087,7 +2038,7 @@
         <v>1.4</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2101,7 +2052,7 @@
         <v>0.8</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2115,7 +2066,7 @@
         <v>1</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2129,7 +2080,7 @@
         <v>1.2</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2143,7 +2094,7 @@
         <v>1.4</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2157,7 +2108,7 @@
         <v>0.8</v>
       </c>
       <c r="D122">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2171,7 +2122,7 @@
         <v>1</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2185,7 +2136,7 @@
         <v>1.2</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2199,7 +2150,7 @@
         <v>1.4</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2213,7 +2164,7 @@
         <v>0.8</v>
       </c>
       <c r="D126">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2227,7 +2178,7 @@
         <v>1</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2241,7 +2192,7 @@
         <v>1.2</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -2255,7 +2206,7 @@
         <v>1.4</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2283,7 +2234,7 @@
         <v>1</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2297,7 +2248,7 @@
         <v>1.2</v>
       </c>
       <c r="D132">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2311,7 +2262,7 @@
         <v>1.4</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -2339,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="D135">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -2353,7 +2304,7 @@
         <v>1.2</v>
       </c>
       <c r="D136">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -2367,7 +2318,7 @@
         <v>1.4</v>
       </c>
       <c r="D137">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -2395,7 +2346,7 @@
         <v>1</v>
       </c>
       <c r="D139">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -2409,7 +2360,7 @@
         <v>1.2</v>
       </c>
       <c r="D140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -2423,7 +2374,7 @@
         <v>1.4</v>
       </c>
       <c r="D141">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -2437,7 +2388,7 @@
         <v>0.8</v>
       </c>
       <c r="D142">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -2451,7 +2402,7 @@
         <v>1</v>
       </c>
       <c r="D143">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -2465,7 +2416,7 @@
         <v>1.2</v>
       </c>
       <c r="D144">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -2479,7 +2430,7 @@
         <v>1.4</v>
       </c>
       <c r="D145">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -2493,7 +2444,7 @@
         <v>0.8</v>
       </c>
       <c r="D146">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -2507,7 +2458,7 @@
         <v>1</v>
       </c>
       <c r="D147">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -2521,7 +2472,7 @@
         <v>1.2</v>
       </c>
       <c r="D148">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -2535,7 +2486,7 @@
         <v>1.4</v>
       </c>
       <c r="D149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -2549,7 +2500,7 @@
         <v>0.8</v>
       </c>
       <c r="D150">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -2563,7 +2514,7 @@
         <v>1</v>
       </c>
       <c r="D151">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -2577,7 +2528,7 @@
         <v>1.2</v>
       </c>
       <c r="D152">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -2591,7 +2542,7 @@
         <v>1.4</v>
       </c>
       <c r="D153">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -2605,7 +2556,7 @@
         <v>0.8</v>
       </c>
       <c r="D154">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -2619,7 +2570,7 @@
         <v>1</v>
       </c>
       <c r="D155">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -2633,7 +2584,7 @@
         <v>1.2</v>
       </c>
       <c r="D156">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -2647,7 +2598,7 @@
         <v>1.4</v>
       </c>
       <c r="D157">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -2661,7 +2612,7 @@
         <v>0.8</v>
       </c>
       <c r="D158">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -2675,7 +2626,7 @@
         <v>1</v>
       </c>
       <c r="D159">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -2689,7 +2640,7 @@
         <v>1.2</v>
       </c>
       <c r="D160">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -2703,7 +2654,7 @@
         <v>1.4</v>
       </c>
       <c r="D161">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -2717,7 +2668,7 @@
         <v>0.8</v>
       </c>
       <c r="D162">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -2731,7 +2682,7 @@
         <v>1</v>
       </c>
       <c r="D163">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -2745,7 +2696,7 @@
         <v>1.2</v>
       </c>
       <c r="D164">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -2759,7 +2710,7 @@
         <v>1.4</v>
       </c>
       <c r="D165">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -2787,7 +2738,7 @@
         <v>1</v>
       </c>
       <c r="D167">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -2801,7 +2752,7 @@
         <v>1.2</v>
       </c>
       <c r="D168">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -2815,7 +2766,7 @@
         <v>1.4</v>
       </c>
       <c r="D169">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2832,6 +2783,5 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated the bulk test excel file
</commit_message>
<xml_diff>
--- a/feasibility_flags_flat.xlsx
+++ b/feasibility_flags_flat.xlsx
@@ -8,22 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atakan\atakan_python\vol_smile_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F07F656-679E-41E5-86BE-AB01B0D9D59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F398D39-F307-4A4E-BEE1-48A9ABCB415D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$169</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>MaturityDays</t>
   </si>
@@ -36,12 +33,15 @@
   <si>
     <t>Flag</t>
   </si>
+  <si>
+    <t>FLAG QNB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +53,21 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,17 +102,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -397,21 +417,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D169"/>
+  <dimension ref="A1:E189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,8 +445,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>30</v>
       </c>
@@ -438,8 +462,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>30</v>
       </c>
@@ -452,8 +479,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>30</v>
       </c>
@@ -466,8 +496,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>30</v>
       </c>
@@ -480,8 +513,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>30</v>
       </c>
@@ -494,8 +530,11 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>30</v>
       </c>
@@ -508,8 +547,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -522,8 +564,11 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>30</v>
       </c>
@@ -536,8 +581,11 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>30</v>
       </c>
@@ -550,8 +598,11 @@
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>30</v>
       </c>
@@ -564,8 +615,11 @@
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>30</v>
       </c>
@@ -578,8 +632,11 @@
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>30</v>
       </c>
@@ -592,8 +649,11 @@
       <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>30</v>
       </c>
@@ -606,8 +666,11 @@
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>30</v>
       </c>
@@ -620,8 +683,11 @@
       <c r="D15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>30</v>
       </c>
@@ -634,8 +700,11 @@
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>30</v>
       </c>
@@ -648,8 +717,11 @@
       <c r="D17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>30</v>
       </c>
@@ -662,8 +734,11 @@
       <c r="D18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>30</v>
       </c>
@@ -676,8 +751,11 @@
       <c r="D19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>30</v>
       </c>
@@ -690,8 +768,11 @@
       <c r="D20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>30</v>
       </c>
@@ -704,8 +785,11 @@
       <c r="D21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>30</v>
       </c>
@@ -718,8 +802,11 @@
       <c r="D22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>30</v>
       </c>
@@ -732,8 +819,11 @@
       <c r="D23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>30</v>
       </c>
@@ -746,8 +836,11 @@
       <c r="D24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>30</v>
       </c>
@@ -760,8 +853,11 @@
       <c r="D25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>30</v>
       </c>
@@ -774,8 +870,11 @@
       <c r="D26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>30</v>
       </c>
@@ -788,8 +887,11 @@
       <c r="D27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>30</v>
       </c>
@@ -802,8 +904,11 @@
       <c r="D28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>30</v>
       </c>
@@ -816,8 +921,11 @@
       <c r="D29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>60</v>
       </c>
@@ -830,8 +938,11 @@
       <c r="D30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>60</v>
       </c>
@@ -844,8 +955,11 @@
       <c r="D31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>60</v>
       </c>
@@ -858,8 +972,11 @@
       <c r="D32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>60</v>
       </c>
@@ -872,8 +989,11 @@
       <c r="D33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>60</v>
       </c>
@@ -886,8 +1006,11 @@
       <c r="D34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>60</v>
       </c>
@@ -900,8 +1023,11 @@
       <c r="D35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>60</v>
       </c>
@@ -914,8 +1040,11 @@
       <c r="D36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>60</v>
       </c>
@@ -928,8 +1057,11 @@
       <c r="D37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>60</v>
       </c>
@@ -942,8 +1074,11 @@
       <c r="D38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>60</v>
       </c>
@@ -956,8 +1091,11 @@
       <c r="D39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>60</v>
       </c>
@@ -970,8 +1108,11 @@
       <c r="D40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>60</v>
       </c>
@@ -984,8 +1125,11 @@
       <c r="D41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>60</v>
       </c>
@@ -998,8 +1142,11 @@
       <c r="D42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>60</v>
       </c>
@@ -1012,8 +1159,11 @@
       <c r="D43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>60</v>
       </c>
@@ -1026,8 +1176,11 @@
       <c r="D44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>60</v>
       </c>
@@ -1040,8 +1193,11 @@
       <c r="D45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>60</v>
       </c>
@@ -1054,8 +1210,11 @@
       <c r="D46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>60</v>
       </c>
@@ -1068,8 +1227,11 @@
       <c r="D47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>60</v>
       </c>
@@ -1082,8 +1244,11 @@
       <c r="D48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>60</v>
       </c>
@@ -1096,8 +1261,11 @@
       <c r="D49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>60</v>
       </c>
@@ -1110,8 +1278,11 @@
       <c r="D50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>60</v>
       </c>
@@ -1124,8 +1295,11 @@
       <c r="D51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>60</v>
       </c>
@@ -1138,8 +1312,11 @@
       <c r="D52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>60</v>
       </c>
@@ -1152,8 +1329,11 @@
       <c r="D53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>60</v>
       </c>
@@ -1166,8 +1346,11 @@
       <c r="D54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>60</v>
       </c>
@@ -1180,8 +1363,11 @@
       <c r="D55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>60</v>
       </c>
@@ -1194,8 +1380,11 @@
       <c r="D56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>60</v>
       </c>
@@ -1208,8 +1397,11 @@
       <c r="D57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>90</v>
       </c>
@@ -1222,8 +1414,11 @@
       <c r="D58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>90</v>
       </c>
@@ -1236,8 +1431,11 @@
       <c r="D59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>90</v>
       </c>
@@ -1250,8 +1448,11 @@
       <c r="D60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>90</v>
       </c>
@@ -1264,8 +1465,11 @@
       <c r="D61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>90</v>
       </c>
@@ -1278,8 +1482,11 @@
       <c r="D62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>90</v>
       </c>
@@ -1292,8 +1499,11 @@
       <c r="D63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>90</v>
       </c>
@@ -1306,8 +1516,11 @@
       <c r="D64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>90</v>
       </c>
@@ -1320,8 +1533,11 @@
       <c r="D65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>90</v>
       </c>
@@ -1334,8 +1550,11 @@
       <c r="D66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>90</v>
       </c>
@@ -1348,8 +1567,11 @@
       <c r="D67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>90</v>
       </c>
@@ -1362,8 +1584,11 @@
       <c r="D68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>90</v>
       </c>
@@ -1376,8 +1601,11 @@
       <c r="D69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>90</v>
       </c>
@@ -1390,8 +1618,11 @@
       <c r="D70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>90</v>
       </c>
@@ -1404,8 +1635,11 @@
       <c r="D71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>90</v>
       </c>
@@ -1418,8 +1652,11 @@
       <c r="D72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>90</v>
       </c>
@@ -1432,8 +1669,11 @@
       <c r="D73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>90</v>
       </c>
@@ -1446,8 +1686,11 @@
       <c r="D74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>90</v>
       </c>
@@ -1460,8 +1703,11 @@
       <c r="D75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>90</v>
       </c>
@@ -1474,8 +1720,11 @@
       <c r="D76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>90</v>
       </c>
@@ -1488,8 +1737,11 @@
       <c r="D77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>90</v>
       </c>
@@ -1502,8 +1754,11 @@
       <c r="D78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>90</v>
       </c>
@@ -1516,8 +1771,11 @@
       <c r="D79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>90</v>
       </c>
@@ -1530,8 +1788,11 @@
       <c r="D80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>90</v>
       </c>
@@ -1544,8 +1805,11 @@
       <c r="D81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>90</v>
       </c>
@@ -1558,8 +1822,11 @@
       <c r="D82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>90</v>
       </c>
@@ -1572,8 +1839,11 @@
       <c r="D83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>90</v>
       </c>
@@ -1586,8 +1856,11 @@
       <c r="D84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>90</v>
       </c>
@@ -1600,8 +1873,11 @@
       <c r="D85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>180</v>
       </c>
@@ -1614,8 +1890,11 @@
       <c r="D86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>180</v>
       </c>
@@ -1628,8 +1907,11 @@
       <c r="D87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>180</v>
       </c>
@@ -1642,8 +1924,11 @@
       <c r="D88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>180</v>
       </c>
@@ -1656,8 +1941,11 @@
       <c r="D89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>180</v>
       </c>
@@ -1670,8 +1958,11 @@
       <c r="D90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>180</v>
       </c>
@@ -1684,8 +1975,11 @@
       <c r="D91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>180</v>
       </c>
@@ -1698,8 +1992,11 @@
       <c r="D92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>180</v>
       </c>
@@ -1712,8 +2009,11 @@
       <c r="D93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>180</v>
       </c>
@@ -1726,8 +2026,11 @@
       <c r="D94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>180</v>
       </c>
@@ -1740,8 +2043,11 @@
       <c r="D95">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>180</v>
       </c>
@@ -1754,8 +2060,11 @@
       <c r="D96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>180</v>
       </c>
@@ -1768,8 +2077,11 @@
       <c r="D97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>180</v>
       </c>
@@ -1782,8 +2094,11 @@
       <c r="D98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>180</v>
       </c>
@@ -1796,8 +2111,11 @@
       <c r="D99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>180</v>
       </c>
@@ -1810,8 +2128,11 @@
       <c r="D100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>180</v>
       </c>
@@ -1824,8 +2145,11 @@
       <c r="D101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>180</v>
       </c>
@@ -1838,8 +2162,11 @@
       <c r="D102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>180</v>
       </c>
@@ -1852,8 +2179,11 @@
       <c r="D103">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>180</v>
       </c>
@@ -1866,8 +2196,11 @@
       <c r="D104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>180</v>
       </c>
@@ -1880,8 +2213,11 @@
       <c r="D105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>180</v>
       </c>
@@ -1894,8 +2230,11 @@
       <c r="D106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>180</v>
       </c>
@@ -1908,8 +2247,11 @@
       <c r="D107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>180</v>
       </c>
@@ -1922,8 +2264,11 @@
       <c r="D108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>180</v>
       </c>
@@ -1936,8 +2281,11 @@
       <c r="D109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>180</v>
       </c>
@@ -1950,8 +2298,11 @@
       <c r="D110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>180</v>
       </c>
@@ -1964,8 +2315,11 @@
       <c r="D111">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>180</v>
       </c>
@@ -1978,8 +2332,11 @@
       <c r="D112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>180</v>
       </c>
@@ -1992,8 +2349,11 @@
       <c r="D113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>270</v>
       </c>
@@ -2006,8 +2366,11 @@
       <c r="D114">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>270</v>
       </c>
@@ -2020,8 +2383,11 @@
       <c r="D115">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>270</v>
       </c>
@@ -2034,8 +2400,11 @@
       <c r="D116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>270</v>
       </c>
@@ -2048,8 +2417,11 @@
       <c r="D117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>270</v>
       </c>
@@ -2062,8 +2434,11 @@
       <c r="D118">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>270</v>
       </c>
@@ -2076,8 +2451,11 @@
       <c r="D119">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>270</v>
       </c>
@@ -2090,8 +2468,11 @@
       <c r="D120">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>270</v>
       </c>
@@ -2104,8 +2485,11 @@
       <c r="D121">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>270</v>
       </c>
@@ -2118,8 +2502,11 @@
       <c r="D122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>270</v>
       </c>
@@ -2132,8 +2519,11 @@
       <c r="D123">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>270</v>
       </c>
@@ -2146,8 +2536,11 @@
       <c r="D124">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>270</v>
       </c>
@@ -2160,8 +2553,11 @@
       <c r="D125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>270</v>
       </c>
@@ -2174,8 +2570,11 @@
       <c r="D126">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>270</v>
       </c>
@@ -2188,8 +2587,11 @@
       <c r="D127">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>270</v>
       </c>
@@ -2202,8 +2604,11 @@
       <c r="D128">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>270</v>
       </c>
@@ -2216,8 +2621,11 @@
       <c r="D129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>270</v>
       </c>
@@ -2230,8 +2638,11 @@
       <c r="D130">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>270</v>
       </c>
@@ -2244,8 +2655,11 @@
       <c r="D131">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>270</v>
       </c>
@@ -2258,8 +2672,11 @@
       <c r="D132">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>270</v>
       </c>
@@ -2272,8 +2689,11 @@
       <c r="D133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>270</v>
       </c>
@@ -2286,8 +2706,11 @@
       <c r="D134">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>270</v>
       </c>
@@ -2300,8 +2723,11 @@
       <c r="D135">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>270</v>
       </c>
@@ -2314,8 +2740,11 @@
       <c r="D136">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>270</v>
       </c>
@@ -2328,8 +2757,11 @@
       <c r="D137">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>270</v>
       </c>
@@ -2342,8 +2774,11 @@
       <c r="D138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>270</v>
       </c>
@@ -2356,8 +2791,11 @@
       <c r="D139">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>270</v>
       </c>
@@ -2370,8 +2808,11 @@
       <c r="D140">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>270</v>
       </c>
@@ -2384,8 +2825,11 @@
       <c r="D141">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>360</v>
       </c>
@@ -2398,8 +2842,11 @@
       <c r="D142">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>360</v>
       </c>
@@ -2412,8 +2859,11 @@
       <c r="D143">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E143" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>360</v>
       </c>
@@ -2426,8 +2876,11 @@
       <c r="D144">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>360</v>
       </c>
@@ -2440,8 +2893,11 @@
       <c r="D145">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>360</v>
       </c>
@@ -2454,8 +2910,11 @@
       <c r="D146">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>360</v>
       </c>
@@ -2468,8 +2927,11 @@
       <c r="D147">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>360</v>
       </c>
@@ -2482,8 +2944,11 @@
       <c r="D148">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E148" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>360</v>
       </c>
@@ -2496,8 +2961,11 @@
       <c r="D149">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E149" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>360</v>
       </c>
@@ -2510,8 +2978,11 @@
       <c r="D150">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E150" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>360</v>
       </c>
@@ -2524,8 +2995,11 @@
       <c r="D151">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E151" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>360</v>
       </c>
@@ -2538,8 +3012,11 @@
       <c r="D152">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E152" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>360</v>
       </c>
@@ -2552,8 +3029,11 @@
       <c r="D153">
         <v>1</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E153" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>360</v>
       </c>
@@ -2566,8 +3046,11 @@
       <c r="D154">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E154" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>360</v>
       </c>
@@ -2580,8 +3063,11 @@
       <c r="D155">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E155" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>360</v>
       </c>
@@ -2594,8 +3080,11 @@
       <c r="D156">
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E156" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>360</v>
       </c>
@@ -2608,8 +3097,11 @@
       <c r="D157">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E157" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>360</v>
       </c>
@@ -2622,8 +3114,11 @@
       <c r="D158">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E158" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>360</v>
       </c>
@@ -2636,8 +3131,11 @@
       <c r="D159">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E159" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>360</v>
       </c>
@@ -2650,8 +3148,11 @@
       <c r="D160">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E160" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>360</v>
       </c>
@@ -2664,8 +3165,11 @@
       <c r="D161">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E161" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>360</v>
       </c>
@@ -2678,8 +3182,11 @@
       <c r="D162">
         <v>1</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E162" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>360</v>
       </c>
@@ -2692,8 +3199,11 @@
       <c r="D163">
         <v>1</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E163" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>360</v>
       </c>
@@ -2706,8 +3216,11 @@
       <c r="D164">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E164" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>360</v>
       </c>
@@ -2720,8 +3233,11 @@
       <c r="D165">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E165" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>360</v>
       </c>
@@ -2734,8 +3250,11 @@
       <c r="D166">
         <v>1</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E166" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>360</v>
       </c>
@@ -2748,8 +3267,11 @@
       <c r="D167">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E167" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>360</v>
       </c>
@@ -2762,8 +3284,11 @@
       <c r="D168">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E168" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>360</v>
       </c>
@@ -2776,10 +3301,84 @@
       <c r="D169">
         <v>0</v>
       </c>
+      <c r="E169" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E170" s="4"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E171" s="4"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E172" s="4"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E173" s="4"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E174" s="4"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E175" s="4"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E176" s="4"/>
+    </row>
+    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E177" s="4"/>
+    </row>
+    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E178" s="4"/>
+    </row>
+    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E179" s="4"/>
+    </row>
+    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E180" s="4"/>
+    </row>
+    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E181" s="4"/>
+    </row>
+    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E182" s="4"/>
+    </row>
+    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E183" s="4"/>
+    </row>
+    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E184" s="4"/>
+    </row>
+    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E185" s="4"/>
+    </row>
+    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E186" s="4"/>
+    </row>
+    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E187" s="4"/>
+    </row>
+    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E188" s="4"/>
+    </row>
+    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E189" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D169" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="D2:D1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>